<commit_message>
Added storing of ratios
</commit_message>
<xml_diff>
--- a/stock-unique-dummy.xlsx
+++ b/stock-unique-dummy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -364,6 +364,72 @@
   </si>
   <si>
     <t>http://www.moneycontrol.com/india/stockpricequote/pharmaceuticals/nathbiogenes/NBG</t>
+  </si>
+  <si>
+    <t>infrastructure-general</t>
+  </si>
+  <si>
+    <t>cement-major</t>
+  </si>
+  <si>
+    <t>hospitals-medical-services</t>
+  </si>
+  <si>
+    <t>auto-lcvs-hcvs</t>
+  </si>
+  <si>
+    <t>paints-varnishes</t>
+  </si>
+  <si>
+    <t>pharmaceuticals</t>
+  </si>
+  <si>
+    <t>banks-private-sector</t>
+  </si>
+  <si>
+    <t>auto-2-3-wheelers</t>
+  </si>
+  <si>
+    <t>finance-leasing-hire-purchase</t>
+  </si>
+  <si>
+    <t>finance-investments</t>
+  </si>
+  <si>
+    <t>banks-public-sector</t>
+  </si>
+  <si>
+    <t>electricals</t>
+  </si>
+  <si>
+    <t>castings-forgings</t>
+  </si>
+  <si>
+    <t>telecommunications-service</t>
+  </si>
+  <si>
+    <t>telecommunications-equipment</t>
+  </si>
+  <si>
+    <t>auto-ancillaries</t>
+  </si>
+  <si>
+    <t>refineries</t>
+  </si>
+  <si>
+    <t>food-processing</t>
+  </si>
+  <si>
+    <t>pesticides-agro-chemicals</t>
+  </si>
+  <si>
+    <t>textiles-composite-mills</t>
+  </si>
+  <si>
+    <t>textiles-denim</t>
+  </si>
+  <si>
+    <t>Industry</t>
   </si>
 </sst>
 </file>
@@ -1156,15 +1222,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1223"/>
+  <dimension ref="A1:K1223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="10" max="10" width="92.89453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,8 +1264,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1227,8 +1299,11 @@
       <c r="J2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1259,8 +1334,11 @@
       <c r="J3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1291,8 +1369,11 @@
       <c r="J4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1323,8 +1404,11 @@
       <c r="J5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1355,8 +1439,11 @@
       <c r="J6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1387,8 +1474,11 @@
       <c r="J7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1419,8 +1509,11 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1451,8 +1544,11 @@
       <c r="J9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1483,8 +1579,11 @@
       <c r="J10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1515,8 +1614,11 @@
       <c r="J11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1547,8 +1649,11 @@
       <c r="J12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1579,8 +1684,11 @@
       <c r="J13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1611,8 +1719,11 @@
       <c r="J14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1643,8 +1754,11 @@
       <c r="J15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1675,8 +1789,11 @@
       <c r="J16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1707,8 +1824,11 @@
       <c r="J17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1739,8 +1859,11 @@
       <c r="J18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1771,8 +1894,11 @@
       <c r="J19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1803,8 +1929,11 @@
       <c r="J20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1835,8 +1964,11 @@
       <c r="J21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1867,8 +1999,11 @@
       <c r="J22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -1899,8 +2034,11 @@
       <c r="J23" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1931,8 +2069,11 @@
       <c r="J24" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -1963,8 +2104,11 @@
       <c r="J25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -1995,8 +2139,11 @@
       <c r="J26" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2027,8 +2174,11 @@
       <c r="J27" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -2059,8 +2209,11 @@
       <c r="J28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2091,14 +2244,17 @@
       <c r="J29" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>

</xml_diff>